<commit_message>
Update databases to match up-to-date formats
The data files in the SLE database were based on an older version of CEA's Singapore-database. This mismatch in database formats could lead to crashes when working with some cases. Updating the database formats to the latest version should fix these issues.

This update will have to be renewed in a few weeks as another big change in the CEA databases is scheduled to be pushed to master soon.
</commit_message>
<xml_diff>
--- a/cea/databases/SG_SLE/archetypes/CONSTRUCTION_STANDARD.xlsx
+++ b/cea/databases/SG_SLE/archetypes/CONSTRUCTION_STANDARD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reynoldmok/Documents/GitHub/CityEnergyAnalyst/cea/databases/SG_SLE/archetypes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Desktop\SG_SLE\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C0A30D-C93F-9C47-B27B-A64122C58D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7090E2A1-F60A-4160-9561-56AE295B7DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="760" windowWidth="33420" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="-16200" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,15 +367,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -402,10 +427,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,260 +766,266 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1000</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>1000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>1000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>1000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>1000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>1000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>1000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>1000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>1000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>1000</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>1000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>1000</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>1000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>1000</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>1000</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>1000</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>2040</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>1000</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>2040</v>
       </c>
     </row>
@@ -976,15 +1036,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.26953125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.1796875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="10.81640625" style="11" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,1006 +1116,1008 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="7">
         <v>0.9</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="7">
         <v>0.25</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
+      <c r="M2" s="8">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="7">
         <v>1</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="7">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="7">
         <v>0.9</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="7">
         <v>0.84</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="7">
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="7">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="U3" s="9"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="7">
         <v>0.9</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="7">
         <v>0.84</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
         <v>0.59</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="7">
         <v>0.59</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="7">
         <v>0.59</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="7">
         <v>0.59</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="7">
         <v>0.9</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="7">
         <v>0.84</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
         <v>1</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
+      <c r="O5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="7">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="7">
         <v>0.9</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="7">
         <v>0.84</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
         <v>1</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
         <v>0.59</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="7">
         <v>0.59</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="7">
         <v>0.59</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="7">
         <v>0.59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="7">
         <v>0.95</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="7">
         <v>0.75</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
         <v>1</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
+      <c r="O7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <v>0.8</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="7">
         <v>0.8</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="7">
         <v>0.8</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="7">
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="7">
         <v>0.8</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="7">
         <v>0.35</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
         <v>0.9</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="7">
         <v>1</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="7">
         <v>0.4</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="7">
         <v>0.4</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="7">
         <v>0.95</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="7">
         <v>0.95</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
         <v>1</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
+      <c r="O9" s="7">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
         <v>0.6</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="7">
         <v>0.6</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="7">
         <v>0.6</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="7">
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="7">
         <v>0.95</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="7">
         <v>0.75</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7">
         <v>1</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
+      <c r="O10" s="7">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
         <v>0.7</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="7">
         <v>0.7</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="7">
         <v>0.7</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="7">
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="7">
         <v>0.95</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="7">
         <v>0.5</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
         <v>1</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="7">
         <v>0.4</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="7">
         <v>0.4</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="7">
         <v>0.8</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="7">
         <v>0.35</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12" s="7">
         <v>0.9</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="7">
         <v>1</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="7">
         <v>0.35</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="7">
         <v>0.35</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="7">
         <v>0.35</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="7">
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="7">
         <v>0.95</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="7">
         <v>0.75</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="7">
         <v>1</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="7">
         <v>0.4</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="7">
         <v>0.4</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="7">
         <v>0.95</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="7">
         <v>0.7</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
+      <c r="M14" s="8">
+        <v>0</v>
+      </c>
+      <c r="N14" s="7">
         <v>1</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
+      <c r="O14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="7">
         <v>0.4</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="7">
         <v>0.4</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="7">
         <v>0.95</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="7">
         <v>0.5</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
+      <c r="M15" s="8">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
         <v>1</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="7">
         <v>0.4</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="7">
         <v>0.4</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="7">
         <v>0.8</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="7">
         <v>0.35</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
+      <c r="M16" s="8">
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
         <v>0.9</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="7">
         <v>1</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="7">
         <v>0.35</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="7">
         <v>0.35</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="7">
         <v>0.35</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="7">
         <v>0.35</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="7">
         <v>0.95</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="7">
         <v>0.75</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
+      <c r="M17" s="8">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
         <v>1</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
+      <c r="O17" s="7">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="7">
         <v>0.4</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="7">
         <v>0.4</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="7">
         <v>0.95</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="7">
         <v>0.7</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
+      <c r="M18" s="8">
+        <v>0</v>
+      </c>
+      <c r="N18" s="7">
         <v>1</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
+      <c r="O18" s="7">
+        <v>0</v>
+      </c>
+      <c r="P18" s="7">
         <v>0.4</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="7">
         <v>0.4</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="7">
         <v>0.4</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="7">
         <v>0.4</v>
       </c>
     </row>
@@ -2053,15 +2128,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J1048558"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2093,549 +2181,552 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="G10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="G12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G13" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="G13" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="G14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="G15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="G16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" t="s">
-        <v>92</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="G17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G18" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="G18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="12" t="s">
         <v>94</v>
       </c>
+    </row>
+    <row r="1048558" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E1048558" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2644,15 +2735,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E1048557"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2669,294 +2768,297 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="1048557" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E1048557" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>